<commit_message>
v1.3 Fix para ofertas de terceros para ignorar cantidades vacias. Otros fixes de errores y excepciones
</commit_message>
<xml_diff>
--- a/basesDeDatos/baseDeDatosParaInforme.xlsx
+++ b/basesDeDatos/baseDeDatosParaInforme.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david.herrera\programmingProjects\automatizacionDocumental\basesDeDatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D174A276-7D9D-45C6-90A3-9708F0DD1637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335D7E4A-3DFE-4858-B5C2-C26D8E58E150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1890" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja" sheetId="1" r:id="rId1"/>
-    <sheet name="Base de datos" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="4" r:id="rId1"/>
+    <sheet name="Hoja3" sheetId="5" r:id="rId2"/>
+    <sheet name="Hoja" sheetId="1" r:id="rId3"/>
+    <sheet name="Base de datos" sheetId="2" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="154">
   <si>
     <t>ITEM</t>
   </si>
@@ -375,6 +377,275 @@
   </si>
   <si>
     <t>11214-00</t>
+  </si>
+  <si>
+    <t>11214-00-001-24-1828</t>
+  </si>
+  <si>
+    <t>11214-00-002-24-1828</t>
+  </si>
+  <si>
+    <t>TERMÓMETRO DIGITAL DE REFERENCIA</t>
+  </si>
+  <si>
+    <t>SISTEMA DE MEDICIÓN DE DBO/ SISTEMA DE MEDICIÓN RESPIROMÉTRICO</t>
+  </si>
+  <si>
+    <t>KIT STEAM DE ROBÓTICA</t>
+  </si>
+  <si>
+    <t>ESTEREOMICROSCOPIO BINOCULAR</t>
+  </si>
+  <si>
+    <t>KIT CAIDA LIBRE</t>
+  </si>
+  <si>
+    <t>HIDRÓMETRO UNIVERSAL</t>
+  </si>
+  <si>
+    <t>KIT DE MODELOS ANATÓMICOS</t>
+  </si>
+  <si>
+    <t>KIT CROMATOGRAFÍA EN COLUMNA</t>
+  </si>
+  <si>
+    <t>KIT CAPACIDAD CALORÍFICA</t>
+  </si>
+  <si>
+    <t>KIT DE MICROPIPETAS ELECTRÓNICAS</t>
+  </si>
+  <si>
+    <t>BALANZA ELECTRÓNICA 3200 G</t>
+  </si>
+  <si>
+    <t>BALANZA ANALITICA 220 G</t>
+  </si>
+  <si>
+    <t>BALANZA DE PRECISIÓN 620 G</t>
+  </si>
+  <si>
+    <t>BALANZA ELECTRÓNICA 6200 G</t>
+  </si>
+  <si>
+    <t>MULTIMETRO PORTATIL</t>
+  </si>
+  <si>
+    <t>VAL-51-24-DOT-INS</t>
+  </si>
+  <si>
+    <t>VAL-02-24-DOT-INS</t>
+  </si>
+  <si>
+    <t>VAL-06-24-DOT-INS</t>
+  </si>
+  <si>
+    <t>VAL-08-24-DOT-INS</t>
+  </si>
+  <si>
+    <t>VAL-55-24-DOT-INS</t>
+  </si>
+  <si>
+    <t>Las cajas del embalaje se encuentran en perfecto estado físico y no presentan signos de golpes o novedades por el transporte. Se encuentran las siguientes referencias: G30 [1000276] SISTEMA CIRCULATORIO HUMANO, G15 [1000270] MODELO DE PULMÓN 7 PIEZAS, K21 [1000307] EL SISTEMA DIGESTIVO 3 PIEZAS, K32 [1000317] SISTEMA URINARIO DE SEXO DUAL 6 PIEZAS, K10/1 [1000297] NEFRONES Y CONDUCTOS SANGUÍNEOS 120 VECES SU TAMAÑO NATURAL, C22 [1000228] CEREBRO NEURO-ANATÓMICO DESMONTABLE 8 PIEZAS, A20/9 [1002162] CRÁNEO CLÁSICO CON CEREBRO, A794 [1000157] COLUMNA VERTEBRAL, A73 [1000145] COLUMNA DORSAL, A74 [1000146] COLUMNA VERTEBRAL DORSAL, A137/1 [1002177] ESQUELETO SAM DE LUJO COLGADO DE PIE METÁLICO DE 5 RUEDAS, H10 [1000281] PELVIS FEMENINA 2 PIEZAS, H11 [1000282] PELVIS MASCULINA 2 PIEZAS, A291 [1023540] CRÁNEO DESMONTABLE 22 PIEZAS, R04 [1000523] CÉLULA ANIMAL, M33/1 [1000358] MODELO DEL ESQUELETO DE LA MANO CON LIGAMENTOS Y MÚSCULOS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se realiza el desempaquetado de los modelos para verificar su integridad física. El embalaje se encuentra en excelente estado. Se realiza el montaje de los modelos en el lugar designado para su uso por la Universidad. Para cada modelo se realiza el desarmado de las piezas, para los cuales aplica, para verificar la integridad física de los acoples de metal de las piezas.
+Se realiza nuevamente el montaje de las piezas de cada modelo para comprobar su correcto armado. Todas las piezas y subaccesorios de cada modelo se encuentran en perfecto estado físico.
+Se realiza la ubicación final de los modelos en el laboratorio de morfofisiología.
+Se realiza las pruebas de la aplicación de realidad aumentada 3B Smart Anatomy. Todas las pruebas son exitosas, mostrando el correcto funcionamiento de la aplicación y el escaneo por parte de la misma a cada uno de los modelos.
+</t>
+  </si>
+  <si>
+    <t>Se recomienda que el laboratorio donde se encuentran ubicados los modelos tenga un ambiente controlado de temperatura y humedad relativa para prolongar la vida útil de los mismos.
+La humedad puede causar oxidación de las piezas metálicas y decoloración del plástico. La presencia de químicos volátiles puede causar corrosión.</t>
+  </si>
+  <si>
+    <t>P2330167</t>
+  </si>
+  <si>
+    <t>Las cajas del embalaje se encuentran en perfecto estado físico y no presentan signos de golpes o novedades por el transporte.  Los accesorios del kit se encuentran completos. El sensor de temperatura se encuentra en perfecto estado estético y se entrega junto con una pila de 3V. El mechero no presenta daños en su cartucho.</t>
+  </si>
+  <si>
+    <t>Se realiza el montaje del experimento de acuerdo a las guías de laboratorio.
+Se realiza la instalación del sensor en el experimento.
+Se comprueba el estado de encendido del sensor exitosamente.
+El sensor transmite datos via bluetooth de forma óptima a la tablet, al celular y al PC.
+El software measureApp muestra funcionamiento óptimo y estable y recibe los datos de forma correcta.
+Se hacen varias pruebas de temperatura para el sensor y el calorímetro. 
+Las curvas de temperatura muestran el comportamiento adiabático del calorímetro de manera exitosa.</t>
+  </si>
+  <si>
+    <t>Se recomienda almacenar los accesorios para eviar extraviarlos.
+Se recomienda almacenar el cartucho de butano y propano en un lugar fresco y lejos de la luz solar. 
+Se recomienda almacenar el sensor de un lugar libre de polvo y humedad, aunque el sensor tiene protección contra el agua IP67, pero la recomendación se da para alargar la vida útil.
+Se recomienda apagar el sensor cuando no esté en uso para conservar la vida útil de la batería. En lo posible desconectar la batería después de usarlo.</t>
+  </si>
+  <si>
+    <t>P1004105 </t>
+  </si>
+  <si>
+    <t>Se realiza el montaje del experimento siguiendo las guías experimentales de la marca.
+Se realiza la instalación del cronómetro 2-1 utilizando la fuente provista.
+El cronómetro enciende correctamente.
+Se hace la instalación de las barreras fotoeléctricas en el montaje y se instalan en el cronómetro.
+Las barreras presentan condiciones funcionales óptimas y esperadas según los valores obtenidos en el cronómetro 2-1.
+Se hacen varias pruebas de lanzamiento obteniendo resultados experimentales esperados.</t>
+  </si>
+  <si>
+    <t>Se recomienda almacenar los equipos en un lugar libre de polvo y humedad.
+Se recomienda desconectar el cronómetro después de su uso. Se recomienda no dejar las barreras fotoeléctricas conectadas en el cronómetro si no están en uso.</t>
+  </si>
+  <si>
+    <t>P3120300 </t>
+  </si>
+  <si>
+    <t>Los accesorios del kit se encuentran en perfectas condiciones. (bases, varillas, nueces y pinzas).
+Las bolas de acero y madera no presentan abolladuras. El disparador se encuentra en buenas condiciones estéticas.
+El cronómetro 2-1 serial: 2303004008 no presenta novedades estéticas y su empaque está en perfecto estado.</t>
+  </si>
+  <si>
+    <t>Los accesorios de vidrio están en perfectas condiciones.
+El marco de experimentos no presenta abolladuras. Está en condiciones óptimas.
+Los reactivos se encuentran en condiciones óptimas, no presentan fugas ni están regados.
+El marco y sus respectivos accesorios están en buen estado</t>
+  </si>
+  <si>
+    <t>Se realizó la verificación del estado de los accesorios de vidrio.
+Se realizó el montaje e instalación del marco de experimentos con todos sus accesorios.
+Se realizó la verificación del estado de los reactivos (almidón y éter de petróleo).
+Se realizó la instalación de la columna de vidrio, erlenmeyer, y botella de vacío, en el tablero (marco de experimentos).
+Se realizó la prueba experimental del experimento propuesto para el montaje.
+Se realizó la instalación de la botella de vacío en punto de agua para su correcto funcionamiento.
+Se realiza posterior limpieza de los elementos.</t>
+  </si>
+  <si>
+    <t>Se recomienda almacenar los accesorios del experimento en un lugar libre de polvo y humedad.
+Se recomienda almacenar los reactivos en mobiliarios dedicados libres de calor y humedad.
+Se recomienda desmontar la vidriería del marco del experimento cuando no esté en uso.
+Se recomienda realizar limpiezas periódicas a los elementos del kit después de cada uso.</t>
+  </si>
+  <si>
+    <t>Laboratorio de Docencia en Física 2do piso</t>
+  </si>
+  <si>
+    <t>9am</t>
+  </si>
+  <si>
+    <t>Mario Quiñonez</t>
+  </si>
+  <si>
+    <t>mario.quinonez@correounivalle.edu.co</t>
+  </si>
+  <si>
+    <t>El embalaje del Péndulo se encuentra en perfecto estado. No se presentan daños o novedades estéticas en el equipo. El eje del motor se encuentra en buen estado y el péndulo de torsión está en buenas condiciones estéticas.</t>
+  </si>
+  <si>
+    <t>Se recomienda almacenar el equipo en un lugar libre de polvo y humedad.
+Desconectar el equipo cuando esté fuera de uso.</t>
+  </si>
+  <si>
+    <t>Se hace la instalación del péndulo en el laboratorio de docencia en física del segundo piso.
+Se hacen pruebas de funcionamiento del motor. El motor funciona bajo los parámetros esperados.
+Se hacen pruebas del electroimán y se encuentra que genera fricción electromagnética según lo esperado.
+El péndulo de torsión gira sin ninguna novedad y se hacen pruebas de ambas prácticas con éxito.</t>
+  </si>
+  <si>
+    <t>Se hace la instalación del péndulo en el laboratorio de docencia en física del segundo piso. Se hacen pruebas de funcionamiento del motor. El motor funciona bajo los parámetros esperados. Se hacen pruebas del electroimán y se encuentra que genera fricción electromagnética según lo esperado. El péndulo presenta una ligera inclinación en su eje lo que causa que tenga fricción mecánica que no es ideal. Se hace el ajuste del eje para arreglar la inclinación del péndulo y se proceden a hacer pruebas de funcionamiento. El péndulo de torsión gira sin ninguna novedad y se hacen pruebas de ambas prácticas con éxito.</t>
+  </si>
+  <si>
+    <t>Los equipos se encuentran en su empaque original sin ningun signo de golpes, rayones o abolladuras. El embalaje se encuentra en buen estado. El equipo balístico (ambos) se encuentra en perfecto estado físico sin ninguna novedad estética. Todas las partes mecánicas se encuentran en buen estado incluyendo la escala angular y los disparadores. Los accesorios del kit se encuentran completos y se entrega todo el conjunto de tornillería y llaves bristol necesarias para el montaje.</t>
+  </si>
+  <si>
+    <t>Se recomienda almacenar los sensores cuando estén fuera de uso. El sensor debe estar desconectado en todo momento mientras que no esté en uso para no afectar su vida útil.
+Se recomienda cuidado con el almacenamiento del péndulo balístico, el cual se entrega en su empaque original para el mismo.
+Se recomienda almacenar los accesorios pequeños como las bolas en un lugar seguro para evitar extraviarlas. 
+Se recomienda no cambiar el computador en el cual se va a utilizar el software. Si se requiere hacer esto último, contactarnos para realizar este procedimiento. También, en caso de requerir instalar el software en más de un computador, lo cual es posible ya que se adquirieron dos licencias.
+Se recomienda almacenar el equipo en un lugar libre de polvo y humedad.
+Se recomienda hacer mantenimiento anual.</t>
+  </si>
+  <si>
+    <t>Salomón Triana</t>
+  </si>
+  <si>
+    <t>salomon.triana@unad.edu.co</t>
+  </si>
+  <si>
+    <t>Se realiza el montaje del experimento siguiendo las guías experimentales de la marca.
+Se realiza la instalación del cronómetro 2-1 utilizando la fuente provista.
+El cronómetro enciende correctamente.
+Se hace la instalación de las barreras fotoeléctricas y los ganchos de disparo en el montaje y se instalan en el cronómetro.
+Las barreras presentan condiciones funcionales óptimas y esperadas según los valores obtenidos en el cronómetro 2-1.
+Se hacen varias pruebas de lanzamiento obteniendo resultados experimentales esperados.</t>
+  </si>
+  <si>
+    <t>2pm</t>
+  </si>
+  <si>
+    <t>3pm</t>
+  </si>
+  <si>
+    <t>4pm</t>
+  </si>
+  <si>
+    <t>Se realiza el desempaquetado de los modelos para verificar su integridad física. El embalaje se encuentra en excelente estado. Se realiza el montaje de los modelos en el lugar designado para su uso por la Universidad. Para cada modelo se realiza el desarmado de las piezas, para los cuales aplica, para verificar la integridad física de los acoples de metal de las piezas.
+Se realiza nuevamente el montaje de las piezas de cada modelo para comprobar su correcto armado. Todas las piezas y subaccesorios de cada modelo se encuentran en perfecto estado físico.
+Se realiza la ubicación final de los modelos en el laboratorio de morfofisiología.
+Se realiza las pruebas de la aplicación de realidad aumentada 3B Smart Anatomy. Todas las pruebas son exitosas, mostrando el correcto funcionamiento de la aplicación y el escaneo por parte de la misma a cada uno de los modelos.</t>
+  </si>
+  <si>
+    <t>Se realizó la verificación del estado de los accesorios de vidrio.
+Se realizó el montaje e instalación del marco de experimentos con todos sus accesorios.
+Se realizó la verificación del estado de los reactivos (almidón y éter de petróleo).
+Se realizó la instalación de la columna de vidrio, erlenmeyer, y botella de vacío, en el tablero (marco de experimentos).
+Se realizó la prueba experimental del experimento propuesto para el montaje.
+Se realizó la instalación del dispositivo de vacío el cual se compone de barómetro, llave de tres vías, válvula y mangueras.
+Se hace la instalación del adaptador provisto para el punto de agua.
+Se hacen pruebas de vacio y se obtienen valores de vacios de hasta -1000mPa según el barómetro provisto.
+Se realiza posterior limpieza de los elementos.</t>
+  </si>
+  <si>
+    <t>Se realiza el montaje del experimento de acuerdo a las guías de laboratorio.
+Se realiza la instalación de los sensores en los calorímetros.
+Se comprueba el estado de encendido del sensor exitosamente.
+El sensor transmite datos via bluetooth de forma óptima a la tablet, al celular y al PC.
+El software measureApp muestra funcionamiento óptimo y estable y recibe los datos de forma correcta.
+Se hacen varias pruebas de temperatura para el sensor y el calorímetro. 
+Las curvas de temperatura muestran el comportamiento adiabático del calorímetro de manera exitosa.
+Se realizan pruebas de funcionamiento del mechero con éxito.</t>
+  </si>
+  <si>
+    <t>Se recomienda almacenar los accesorios para eviar extraviarlos.
+Se recomienda almacenar el cartucho de butano y propano en un lugar fresco y lejos de la luz solar. 
+Se recomienda almacenar ambos sensores en un lugar libre de polvo y humedad, aunque el sensor tiene protección contra el agua IP67, pero la recomendación se da para alargar la vida útil.
+Se recomienda apagar el sensor cuando no esté en uso para conservar la vida útil de la batería. En lo posible desconectar la batería después de usarlo.</t>
+  </si>
+  <si>
+    <t>Laboratorio Multipropósito 4</t>
+  </si>
+  <si>
+    <t>Laboratorio Multipropósito 1</t>
+  </si>
+  <si>
+    <t>Laboratorio Multipropósito 2</t>
+  </si>
+  <si>
+    <t>Se realiza el desembalaje del kit para comprobar su estado inicial después del transporte. Se realiza una verificación del volumen de suministro de ambos kits para verificar la integridad de cada accesorio y la completitud de estos. Todos los accesorios se encuentran intactos. 
+Se realiza la instalación de ambas bases de la Unidad Balística con la tornillería y llave bristol provista. Se realiza la instalación de los sensores de velocidad en cada Unidad usando la tornillería provista. Se instalan las escala en el pié cónico. 
+Se hacen pruebas de las compuertas fotoeléctricas de los sensores de velocidad utilizando mediciones manuales y lanzamientos del disparador en 3 niveles. 
+Se hace la instalación de ambos péndulos balísticos en cada unidad y se realizan pruebas de lanzamiento de este para comprobar el funcionamiento mecánico de la trampa de proyectiles, los cuales demuestran funcionamiento óptimo. El indicador de altura del péndulo también funciona según lo esperado.
+Por último, se realiza la instalación del software MeasureDynamics en el computador provisto por la Universidad. Se entregan dos licencias con códigos: 92400121-440-12013751 y 92400121-440-11791441 respectivamente. La segunda licencia se instala a solicitud de un profesor en el computador que usa en el laboratorio.
+Sin embargo, el coordinador indica que no hay un computador asignado para el laboratorio por lo que el software es instalado en un computador provisional. Se realizan pruebas de funcionamiento del software con videos tomados en un smartphone. El algoritmo de conversión y compresión de videos funcionan correctamente, y el análisis de video funciona perfectamente bajo parámetros recomendados.
+En general, el funcionamiento de todo el kit es óptimo y está listo para su uso.</t>
+  </si>
+  <si>
+    <t>10am</t>
+  </si>
+  <si>
+    <t>Las cajas del embalaje se encuentran en perfecto estado físico y no presentan signos de golpes o novedades por el transporte.  Los accesorios del kit se encuentran completos. Los sensores (2) de temperatura se encuentran en perfecto estado estético y se entregan junto con una pila de 3V. Los seriales de los sensores son C00011E88 y C000147B2. Los mecheros no presentan daños en su cartucho.</t>
+  </si>
+  <si>
+    <t>Los accesorios del kit se encuentran en perfectas condiciones. (bases, varillas, nueces y pinzas).
+Las bolas de acero y madera no presentan abolladuras. El disparador se encuentra en buenas condiciones estéticas.
+Los cronómetros 2-1 serial: 2303004008 y 2303004009 no presentan novedades estéticas y su empaque está en perfecto estado.</t>
   </si>
 </sst>
 </file>
@@ -729,12 +1000,541 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{655EC420-93C8-4D5F-8A9C-EAA108D1F7F6}">
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T4" sqref="T4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" customWidth="1"/>
+    <col min="18" max="18" width="20.85546875" customWidth="1"/>
+    <col min="20" max="20" width="79.5703125" customWidth="1"/>
+    <col min="21" max="21" width="149.28515625" customWidth="1"/>
+    <col min="22" max="22" width="104.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="63" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" s="2" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="3">
+        <v>45911</v>
+      </c>
+      <c r="N2" s="3">
+        <v>45546</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="S2" s="2">
+        <v>3218284227</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>68</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>"VAL-" &amp;A3&amp;"-24-DOT-INS"</f>
+        <v>VAL-68-24-DOT-INS</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="3">
+        <v>45911</v>
+      </c>
+      <c r="N3" s="3">
+        <v>45546</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="S3" s="2">
+        <v>3218284227</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>76</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <f t="shared" ref="B4:B7" si="0">"VAL-" &amp;A4&amp;"-24-DOT-INS"</f>
+        <v>VAL-76-24-DOT-INS</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="3">
+        <v>45911</v>
+      </c>
+      <c r="N4" s="3">
+        <v>45546</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="S4" s="2">
+        <v>3218284227</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" s="2" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>86</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>VAL-86-24-DOT-INS</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="3">
+        <v>45911</v>
+      </c>
+      <c r="N5" s="3">
+        <v>45546</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="S5" s="2">
+        <v>3218284227</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" s="2" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>89</v>
+      </c>
+      <c r="B6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>VAL-89-24-DOT-INS</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="3">
+        <v>45911</v>
+      </c>
+      <c r="N6" s="3">
+        <v>45546</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="S6" s="2">
+        <v>3218284227</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>109</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>VAL-109-24-DOT-INS</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="3">
+        <v>45911</v>
+      </c>
+      <c r="N7" s="3">
+        <v>45546</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="S7" s="2">
+        <v>3218284227</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="R2" r:id="rId1" xr:uid="{F8E6D1E9-1553-474E-9800-4CD0D2FB6D00}"/>
+    <hyperlink ref="R3" r:id="rId2" xr:uid="{CB065325-FC8A-4B84-982F-D2E5C4D9B07A}"/>
+    <hyperlink ref="R4" r:id="rId3" xr:uid="{E6C96CF0-7437-4744-86FB-C5F11706C7FB}"/>
+    <hyperlink ref="R5" r:id="rId4" xr:uid="{488B5BF3-DF13-496D-8E0D-502E63BDD5BF}"/>
+    <hyperlink ref="R6" r:id="rId5" xr:uid="{EC217399-1EC2-4A05-8383-4C537895C6F3}"/>
+    <hyperlink ref="R7" r:id="rId6" xr:uid="{EF5170FB-195D-4145-9B1F-2192CD59D509}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A8D869-269F-4B37-913A-B9EA52856E7A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V20"/>
+  <sheetViews>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,7 +1543,7 @@
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="41.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
     <col min="7" max="7" width="23.85546875" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" customWidth="1"/>
@@ -833,12 +1633,14 @@
     </row>
     <row r="2" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
@@ -863,33 +1665,47 @@
       <c r="L2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="6">
-        <v>45899</v>
-      </c>
-      <c r="N2" s="6">
-        <v>45534</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>83</v>
+      <c r="M2" s="3">
+        <v>45910</v>
+      </c>
+      <c r="N2" s="3">
+        <v>45545</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-    </row>
-    <row r="3" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="S2" s="2">
+        <v>3108217426</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
@@ -914,26 +1730,47 @@
       <c r="L3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="6">
-        <v>45899</v>
-      </c>
-      <c r="N3" s="6">
-        <v>45534</v>
+      <c r="M3" s="3">
+        <v>45910</v>
+      </c>
+      <c r="N3" s="3">
+        <v>45545</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="S3" s="2">
+        <v>3108217426</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="G4" s="2"/>
@@ -949,18 +1786,410 @@
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
     </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="240" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>68</v>
+      </c>
+      <c r="B9" t="str">
+        <f>"VAL-" &amp;A9&amp;"-24-DOT-INS"</f>
+        <v>VAL-68-24-DOT-INS</v>
+      </c>
+      <c r="C9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" t="s">
+        <v>28</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>76</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" ref="B10:B20" si="0">"VAL-" &amp;A10&amp;"-24-DOT-INS"</f>
+        <v>VAL-76-24-DOT-INS</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>80</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>VAL-80-24-DOT-INS</v>
+      </c>
+      <c r="C11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="210" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>86</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>VAL-86-24-DOT-INS</v>
+      </c>
+      <c r="C12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="120" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>89</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>VAL-89-24-DOT-INS</v>
+      </c>
+      <c r="C13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" t="s">
+        <v>28</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="120" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>109</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>VAL-109-24-DOT-INS</v>
+      </c>
+      <c r="C14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" t="s">
+        <v>115</v>
+      </c>
+      <c r="G14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>113</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>VAL-113-24-DOT-INS</v>
+      </c>
+      <c r="C15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>183</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>VAL-183-24-DOT-INS</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>187</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>VAL-187-24-DOT-INS</v>
+      </c>
+      <c r="C17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>188</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>VAL-188-24-DOT-INS</v>
+      </c>
+      <c r="C18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>189</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>VAL-189-24-DOT-INS</v>
+      </c>
+      <c r="C19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>199</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>VAL-199-24-DOT-INS</v>
+      </c>
+      <c r="C20" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="R3" r:id="rId1" xr:uid="{4AF0BF26-BF9A-4D7D-A4D9-D053EA8BA2BF}"/>
+    <hyperlink ref="R2" r:id="rId2" xr:uid="{A1EB34BD-0937-4458-9008-C393DAC213D7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B72208-97E1-4C7D-8DC1-CBFEC37313FA}">
   <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2:S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,27 +2323,9 @@
       <c r="L2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="3">
-        <v>45866</v>
-      </c>
-      <c r="N2" s="3">
-        <v>45501</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>33</v>
-      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="R2" s="4"/>
       <c r="T2" s="2" t="s">
         <v>40</v>
       </c>
@@ -1582,15 +2793,131 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="R2" r:id="rId1" xr:uid="{966825D9-3FED-43BD-8665-9B4F728B11C7}"/>
-    <hyperlink ref="R3" r:id="rId2" xr:uid="{3CB7FBBF-8323-4C2C-B387-567B65EB6E90}"/>
-    <hyperlink ref="R4" r:id="rId3" xr:uid="{D717C4D2-78C2-4CC9-9A56-01F414EE5865}"/>
-    <hyperlink ref="R5" r:id="rId4" xr:uid="{4F08A92E-B411-410A-9FDD-95580BF43D6B}"/>
-    <hyperlink ref="R6" r:id="rId5" xr:uid="{A12DBC3C-C657-4569-AB02-5B836CF0649C}"/>
-    <hyperlink ref="R7" r:id="rId6" xr:uid="{3189892B-AC49-4B9C-BC6A-C75F8674D3C4}"/>
-    <hyperlink ref="R8" r:id="rId7" xr:uid="{3FF560E3-7526-4BF1-80FC-F15FCB89C23D}"/>
-    <hyperlink ref="R9" r:id="rId8" xr:uid="{7A755707-CA23-42B4-8F8F-A1C281B90C9C}"/>
+    <hyperlink ref="R3" r:id="rId1" xr:uid="{3CB7FBBF-8323-4C2C-B387-567B65EB6E90}"/>
+    <hyperlink ref="R4" r:id="rId2" xr:uid="{D717C4D2-78C2-4CC9-9A56-01F414EE5865}"/>
+    <hyperlink ref="R5" r:id="rId3" xr:uid="{4F08A92E-B411-410A-9FDD-95580BF43D6B}"/>
+    <hyperlink ref="R6" r:id="rId4" xr:uid="{A12DBC3C-C657-4569-AB02-5B836CF0649C}"/>
+    <hyperlink ref="R7" r:id="rId5" xr:uid="{3189892B-AC49-4B9C-BC6A-C75F8674D3C4}"/>
+    <hyperlink ref="R8" r:id="rId6" xr:uid="{3FF560E3-7526-4BF1-80FC-F15FCB89C23D}"/>
+    <hyperlink ref="R9" r:id="rId7" xr:uid="{7A755707-CA23-42B4-8F8F-A1C281B90C9C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4FA336E-1EB2-45D2-B188-090D4D518930}">
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:21" ht="105" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="6">
+        <v>45899</v>
+      </c>
+      <c r="M1" s="6">
+        <v>45534</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+    </row>
+    <row r="2" spans="1:21" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="6">
+        <v>45899</v>
+      </c>
+      <c r="M2" s="6">
+        <v>45534</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
v1.3.4 Arreglo en Informe
</commit_message>
<xml_diff>
--- a/basesDeDatos/baseDeDatosParaInforme.xlsx
+++ b/basesDeDatos/baseDeDatosParaInforme.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david.herrera\programmingProjects\automatizacionDocumental\basesDeDatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david.herrera\Proyectos_Codigos\automatizacionDocumental\basesDeDatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335D7E4A-3DFE-4858-B5C2-C26D8E58E150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A9BCAF-877E-48F6-9153-66546437B144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="184">
   <si>
     <t>ITEM</t>
   </si>
@@ -569,14 +569,6 @@
     <t>salomon.triana@unad.edu.co</t>
   </si>
   <si>
-    <t>Se realiza el montaje del experimento siguiendo las guías experimentales de la marca.
-Se realiza la instalación del cronómetro 2-1 utilizando la fuente provista.
-El cronómetro enciende correctamente.
-Se hace la instalación de las barreras fotoeléctricas y los ganchos de disparo en el montaje y se instalan en el cronómetro.
-Las barreras presentan condiciones funcionales óptimas y esperadas según los valores obtenidos en el cronómetro 2-1.
-Se hacen varias pruebas de lanzamiento obteniendo resultados experimentales esperados.</t>
-  </si>
-  <si>
     <t>2pm</t>
   </si>
   <si>
@@ -625,27 +617,160 @@
     <t>Laboratorio Multipropósito 1</t>
   </si>
   <si>
+    <t>10am</t>
+  </si>
+  <si>
+    <t>Las cajas del embalaje se encuentran en perfecto estado físico y no presentan signos de golpes o novedades por el transporte.  Los accesorios del kit se encuentran completos. Los sensores (2) de temperatura se encuentran en perfecto estado estético y se entregan junto con una pila de 3V. Los seriales de los sensores son C00011E88 y C000147B2. Los mecheros no presentan daños en su cartucho.</t>
+  </si>
+  <si>
+    <t>MULTÍMETRO DIGITAL DE REFERENCIA</t>
+  </si>
+  <si>
+    <t>INCUBADORA 161 L</t>
+  </si>
+  <si>
+    <t>CABINA DE SEGURIDAD BIOLÓGICA</t>
+  </si>
+  <si>
+    <t>4:30pm</t>
+  </si>
+  <si>
+    <t>leidy.castillo@unad.edu.co</t>
+  </si>
+  <si>
+    <t>Los accesorios del kit se encuentran en perfectas condiciones. (bases, varillas, nueces y pinzas).
+Las bolas de acero y madera no presentan abolladuras. El disparador se encuentra en buenas condiciones estéticas.
+Los cronómetros 2-1 serial: 2303004005 y 2303004063 no presentan novedades estéticas y su empaque está en perfecto estado. 
+Ambas barreras fotoeléctricas se encuentran en su empaque sin novedades estéticas.</t>
+  </si>
+  <si>
+    <t>Se realiza el montaje del experimento siguiendo las guías experimentales de la marca.
+Se realiza la instalación de los cronómetros 2-1 utilizando las fuentes de 5V DC provistas.
+El cronómetro enciende correctamente.
+Se hace la instalación de las barreras fotoeléctricas y los ganchos de disparo en el montaje y se instalan en el cronómetro.
+Las barreras presentan condiciones funcionales óptimas y esperadas según los valores obtenidos en el cronómetro 2-1.
+Se hacen varias pruebas de lanzamiento obteniendo resultados experimentales para los tiempos de caida de la pelora menores a un segundo, lo cual es lo esperado.
+Midiendo la distancia entre los ganchos de disparo y la fotobarrera se hacen pruebas y cálculos de la constante de gravedad obteniendo en promedio un valor de 9.69m/s^2</t>
+  </si>
+  <si>
+    <t>FLUKE</t>
+  </si>
+  <si>
+    <t>El multímetro se encuentra en su empaque sin novedades estéticas de transporte.
+El multímetro no presenta rayones, golpes o hendiduras. 
+Los accesorios se encuentran completos.
+Los accesorios se encuentran no presentan novedades estéticas.</t>
+  </si>
+  <si>
+    <t>Se hace el desempaquetado del multímetro para su comprobación visual y completitud de accesorios.
+Se hace la comprobación de encendido del multímetro.
+El multímetro enciende correctamente y todos sus modos de operación son presentados en la interfaz de manera satisfactoria.
+Se hace la comprobación de funcionamiento de los cables midiendo el voltaje proveniente de una fuente DC y de el tomacorriente AC.
+Los cables transmiten la medición sin novedades.
+Se hace la comprobación funcional de la termocupla para medición de temperatura, con la que se mide la temperatura ambiente de 31°C.</t>
+  </si>
+  <si>
+    <t>Se recomienda almacenar el equipo en su caja cuando esté fuera de funcionamiento.
+Se recomienda almancenarlo en un lugar libre de polvo y humedad.
+Se recomienda leer las instrucciones y el manual de operación para evitar sobrecargas.
+Conectar las entradas del multímetro correspondientes a la corriente máxima que se va a medir.</t>
+  </si>
+  <si>
+    <t>67.1</t>
+  </si>
+  <si>
+    <t>67.2</t>
+  </si>
+  <si>
+    <t>67.3</t>
+  </si>
+  <si>
+    <t>Laboratorio Multipropósito 3</t>
+  </si>
+  <si>
     <t>Laboratorio Multipropósito 2</t>
+  </si>
+  <si>
+    <t>La cabina se encuentra en el laboratorio sin fuera de la caja pero sin instalación previa.
+No presenta novedades estéticas como rayones o hendiduras.
+El vidrio se encuentra en perfecto estado.
+La base se encuentra embalada y no presenta novedades estéticas</t>
+  </si>
+  <si>
+    <t>MEMMERT</t>
+  </si>
+  <si>
+    <t>TOPAIR</t>
+  </si>
+  <si>
+    <t>BO-120-PP</t>
+  </si>
+  <si>
+    <t>21-455630</t>
+  </si>
+  <si>
+    <t>IN60</t>
+  </si>
+  <si>
+    <t>D521.0021</t>
+  </si>
+  <si>
+    <t>1:30pm</t>
+  </si>
+  <si>
+    <t>87V-MAX</t>
+  </si>
+  <si>
+    <t>La base entregada no es la base original por lo que se deja el reporte a Electroequipos para tramitar la garantía de dicha base.
+Se utiliza, por ende, la base de una cabina que está fuera de servicio en la sede.Se hace el montaje en dicha base, que provee mayor seguridad para el equipo y para el personal que opere el equipo.
+Se atornilla la base a la cabina y se ubica en el lugar designado de operación en el laboratorio.
+Se conecta la cabina a la toma eléctrica de 120V y se verifica su estado funcional.
+Se hacen pruebas del extractor exitósamente.
+El motor de subida y bajada del vidrio funciona correctamente sin novedades eléctricas ni mecánicas.
+Las lámparas de iluminación y UltraVioleta funcionan correctamente.
+El sistema de seguridad funciona según lo esperado. Alumbra de color rojo cuando se intenta encender el extractor o la lámpara UV con el vidrio abierto.
+Se concluye el perfecto estado funcional de la cabina de bioseguridad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se recomienda desconectar la Cabina cuando no esté en uso.
+Se recomienda estríctamente no almacenar bebidas ni alimentos comúnes en la cabina.
+No utilizar la iluminación ultravioleta si el vidrio no está cerrado.
+Para subir y bajar el vidrio se debe utilizar el controlador externo (parte derecha).
+</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>Equipo pendiente de instalación</t>
+  </si>
+  <si>
+    <t>El equipo se encuentra en el laboratorio ya desempaquetado y puesto en el lugar dispuesto para su instalación. Se encuentra en perfectas condiciones estéticas y no presenta abolladuras ni rayones.
+El cable se encuentra en perfecto estado estético.
+La incubadora no enciende después de conectada.</t>
+  </si>
+  <si>
+    <t>Se realiza la conexión del cable de poder de la incubadora.
+Al evidenciar que no enciende, se realiza apertura del equipo para revisar la electrónica interna.
+Después de varias verificaciones se encuentra que no hay contacto en dos de los fusibles.
+Se hace una conexión en puente con cable de cobre en lugar de los fusibles para verificar el correcto funcionamiento de la incubadora .
+La incubadora funciona con el puente de manera óptima. Se hace la desconexión de dichos puentes para evitar futuros daños por novedades eléctricas.</t>
+  </si>
+  <si>
+    <t>Electroequipos queda pendiente de hacer el reemplazo de los fusibles para que la incubadora funcione correctamente.
+Se recomienda no operar la incubadora por el momento.</t>
   </si>
   <si>
     <t>Se realiza el desembalaje del kit para comprobar su estado inicial después del transporte. Se realiza una verificación del volumen de suministro de ambos kits para verificar la integridad de cada accesorio y la completitud de estos. Todos los accesorios se encuentran intactos. 
 Se realiza la instalación de ambas bases de la Unidad Balística con la tornillería y llave bristol provista. Se realiza la instalación de los sensores de velocidad en cada Unidad usando la tornillería provista. Se instalan las escala en el pié cónico. 
 Se hacen pruebas de las compuertas fotoeléctricas de los sensores de velocidad utilizando mediciones manuales y lanzamientos del disparador en 3 niveles. 
 Se hace la instalación de ambos péndulos balísticos en cada unidad y se realizan pruebas de lanzamiento de este para comprobar el funcionamiento mecánico de la trampa de proyectiles, los cuales demuestran funcionamiento óptimo. El indicador de altura del péndulo también funciona según lo esperado.
-Por último, se realiza la instalación del software MeasureDynamics en el computador provisto por la Universidad. Se entregan dos licencias con códigos: 92400121-440-12013751 y 92400121-440-11791441 respectivamente. La segunda licencia se instala a solicitud de un profesor en el computador que usa en el laboratorio.
-Sin embargo, el coordinador indica que no hay un computador asignado para el laboratorio por lo que el software es instalado en un computador provisional. Se realizan pruebas de funcionamiento del software con videos tomados en un smartphone. El algoritmo de conversión y compresión de videos funcionan correctamente, y el análisis de video funciona perfectamente bajo parámetros recomendados.
+Por último, se realiza la instalación del software MeasureDynamics en el computador provisto por la Universidad. Se entregan dos licencias con códigos: 92400121-440-17991601 y 92400121-440-16135891.
+ El algoritmo de conversión y compresión de videos funcionan correctamente, y el análisis de video funciona perfectamente bajo parámetros recomendados.
 En general, el funcionamiento de todo el kit es óptimo y está listo para su uso.</t>
   </si>
   <si>
-    <t>10am</t>
-  </si>
-  <si>
-    <t>Las cajas del embalaje se encuentran en perfecto estado físico y no presentan signos de golpes o novedades por el transporte.  Los accesorios del kit se encuentran completos. Los sensores (2) de temperatura se encuentran en perfecto estado estético y se entregan junto con una pila de 3V. Los seriales de los sensores son C00011E88 y C000147B2. Los mecheros no presentan daños en su cartucho.</t>
-  </si>
-  <si>
-    <t>Los accesorios del kit se encuentran en perfectas condiciones. (bases, varillas, nueces y pinzas).
-Las bolas de acero y madera no presentan abolladuras. El disparador se encuentra en buenas condiciones estéticas.
-Los cronómetros 2-1 serial: 2303004008 y 2303004009 no presentan novedades estéticas y su empaque está en perfecto estado.</t>
+    <t>Leidy Castillo</t>
   </si>
 </sst>
 </file>
@@ -704,7 +829,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -720,6 +845,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1001,31 +1129,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{655EC420-93C8-4D5F-8A9C-EAA108D1F7F6}">
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T4" sqref="T4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" customWidth="1"/>
+    <col min="3" max="3" width="20.453125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" customWidth="1"/>
-    <col min="18" max="18" width="20.85546875" customWidth="1"/>
-    <col min="20" max="20" width="79.5703125" customWidth="1"/>
-    <col min="21" max="21" width="149.28515625" customWidth="1"/>
-    <col min="22" max="22" width="104.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.1796875" customWidth="1"/>
+    <col min="9" max="9" width="18.7265625" customWidth="1"/>
+    <col min="10" max="10" width="18.81640625" customWidth="1"/>
+    <col min="11" max="11" width="19.26953125" customWidth="1"/>
+    <col min="12" max="12" width="20.26953125" customWidth="1"/>
+    <col min="17" max="17" width="11.54296875" customWidth="1"/>
+    <col min="18" max="18" width="20.81640625" customWidth="1"/>
+    <col min="20" max="20" width="79.54296875" customWidth="1"/>
+    <col min="21" max="21" width="149.26953125" customWidth="1"/>
+    <col min="22" max="22" width="104.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="63" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="63" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1093,18 +1221,19 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="2" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" s="2" customFormat="1" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>51</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>107</v>
+      <c r="B2" s="2" t="str">
+        <f>"CAR-" &amp;A2&amp;"-24-DOT-INS"</f>
+        <v>CAR-51-24-DOT-INS</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>22</v>
@@ -1131,49 +1260,49 @@
         <v>28</v>
       </c>
       <c r="M2" s="3">
-        <v>45911</v>
+        <v>45924</v>
       </c>
       <c r="N2" s="3">
-        <v>45546</v>
+        <v>45559</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>30</v>
+        <v>148</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>38</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>137</v>
+        <v>183</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="S2" s="2">
-        <v>3218284227</v>
+        <v>3042439787</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>135</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>150</v>
+        <v>182</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" s="2" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>68</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f>"VAL-" &amp;A3&amp;"-24-DOT-INS"</f>
-        <v>VAL-68-24-DOT-INS</v>
+        <f t="shared" ref="B3:B8" si="0">"CAR-" &amp;A3&amp;"-24-DOT-INS"</f>
+        <v>CAR-68-24-DOT-INS</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>96</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>22</v>
@@ -1200,55 +1329,58 @@
         <v>28</v>
       </c>
       <c r="M3" s="3">
-        <v>45911</v>
+        <v>45924</v>
       </c>
       <c r="N3" s="3">
-        <v>45546</v>
+        <v>45559</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>38</v>
+        <v>139</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>137</v>
+        <v>183</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="S3" s="2">
-        <v>3218284227</v>
+        <v>3042439787</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="V3" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>76</v>
+    <row r="4" spans="1:22" s="2" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>161</v>
       </c>
       <c r="B4" s="2" t="str">
-        <f t="shared" ref="B4:B7" si="0">"VAL-" &amp;A4&amp;"-24-DOT-INS"</f>
-        <v>VAL-76-24-DOT-INS</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>65</v>
+        <f t="shared" si="0"/>
+        <v>CAR-67.1-24-DOT-INS</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>150</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>67</v>
+        <v>157</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>72</v>
+        <v>174</v>
+      </c>
+      <c r="G4" s="2">
+        <v>65500090</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>23</v>
@@ -1257,76 +1389,76 @@
         <v>23</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="M4" s="3">
-        <v>45911</v>
+        <v>45924</v>
       </c>
       <c r="N4" s="3">
-        <v>45546</v>
+        <v>45559</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>137</v>
+        <v>183</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="S4" s="2">
-        <v>3218284227</v>
+        <v>3042439787</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>69</v>
+        <v>158</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>70</v>
+        <v>159</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" s="2" customFormat="1" ht="195" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>86</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" s="2" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>162</v>
       </c>
       <c r="B5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>VAL-86-24-DOT-INS</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>98</v>
+        <v>CAR-67.2-24-DOT-INS</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>150</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>51</v>
+        <v>157</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>27</v>
+        <v>174</v>
+      </c>
+      <c r="G5" s="2">
+        <v>65500092</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>23</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>23</v>
@@ -1335,67 +1467,67 @@
         <v>28</v>
       </c>
       <c r="M5" s="3">
-        <v>45911</v>
+        <v>45925</v>
       </c>
       <c r="N5" s="3">
-        <v>45546</v>
+        <v>45560</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>140</v>
+        <v>38</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>137</v>
+        <v>183</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="S5" s="2">
-        <v>3218284227</v>
+        <v>3042439787</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>112</v>
+        <v>158</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" s="2" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>89</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" s="2" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>163</v>
       </c>
       <c r="B6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>VAL-89-24-DOT-INS</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>99</v>
+        <v>CAR-67.3-24-DOT-INS</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>150</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>147</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>22</v>
+        <v>157</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>27</v>
+        <v>174</v>
+      </c>
+      <c r="G6" s="2">
+        <v>65350040</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>23</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>23</v>
@@ -1404,113 +1536,270 @@
         <v>28</v>
       </c>
       <c r="M6" s="3">
-        <v>45911</v>
+        <v>45925</v>
       </c>
       <c r="N6" s="3">
-        <v>45546</v>
+        <v>45560</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>137</v>
+        <v>183</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="S6" s="2">
-        <v>3218284227</v>
+        <v>3042439787</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>109</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" s="2" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="7">
+        <v>69</v>
       </c>
       <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>VAL-109-24-DOT-INS</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>100</v>
+        <v>CAR-69-24-DOT-INS</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>151</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>22</v>
+        <v>167</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>115</v>
+        <v>171</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>27</v>
+        <v>172</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>23</v>
+        <v>177</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>23</v>
+        <v>177</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="L7" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M7" s="3">
+        <v>45925</v>
+      </c>
+      <c r="N7" s="3">
+        <v>45560</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="S7" s="2">
+        <v>3042439787</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="145" x14ac:dyDescent="0.35">
+      <c r="A8" s="7">
+        <v>117</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>CAR-117-24-DOT-INS</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G8" t="s">
+        <v>170</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="3">
-        <v>45911</v>
-      </c>
-      <c r="N7" s="3">
-        <v>45546</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="R7" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="S7" s="2">
-        <v>3218284227</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>146</v>
-      </c>
+      <c r="M8" s="3">
+        <v>45925</v>
+      </c>
+      <c r="N8" s="3">
+        <v>45560</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="S8" s="2">
+        <v>3042439787</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B37" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="R2" r:id="rId1" xr:uid="{F8E6D1E9-1553-474E-9800-4CD0D2FB6D00}"/>
-    <hyperlink ref="R3" r:id="rId2" xr:uid="{CB065325-FC8A-4B84-982F-D2E5C4D9B07A}"/>
-    <hyperlink ref="R4" r:id="rId3" xr:uid="{E6C96CF0-7437-4744-86FB-C5F11706C7FB}"/>
-    <hyperlink ref="R5" r:id="rId4" xr:uid="{488B5BF3-DF13-496D-8E0D-502E63BDD5BF}"/>
-    <hyperlink ref="R6" r:id="rId5" xr:uid="{EC217399-1EC2-4A05-8383-4C537895C6F3}"/>
-    <hyperlink ref="R7" r:id="rId6" xr:uid="{EF5170FB-195D-4145-9B1F-2192CD59D509}"/>
+    <hyperlink ref="R3" r:id="rId2" xr:uid="{52F1C42E-D920-4F2E-BC75-49B0555CD2F7}"/>
+    <hyperlink ref="R4" r:id="rId3" xr:uid="{AA28332A-5A72-4F1B-915C-1D59FC4B1516}"/>
+    <hyperlink ref="R5" r:id="rId4" xr:uid="{AAB82298-B14E-4984-9FFB-C1BEB7E5C1CC}"/>
+    <hyperlink ref="R6" r:id="rId5" xr:uid="{D0EBCE4C-E78A-4891-B7C4-91EA4F281AD0}"/>
+    <hyperlink ref="R7" r:id="rId6" xr:uid="{23599907-B198-44F5-8B30-C65E900ECF7A}"/>
+    <hyperlink ref="R8" r:id="rId7" xr:uid="{D0023600-EDFF-42FE-A2EC-C9DB695A7F60}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1522,7 +1811,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1532,38 +1821,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:V20"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="41.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="41.81640625" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" customWidth="1"/>
+    <col min="7" max="7" width="23.81640625" customWidth="1"/>
+    <col min="8" max="8" width="18.26953125" customWidth="1"/>
+    <col min="9" max="9" width="25.7265625" customWidth="1"/>
+    <col min="10" max="10" width="16.81640625" customWidth="1"/>
+    <col min="11" max="11" width="18.453125" customWidth="1"/>
     <col min="12" max="12" width="33" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" customWidth="1"/>
-    <col min="17" max="17" width="23.28515625" customWidth="1"/>
-    <col min="18" max="18" width="30.5703125" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" customWidth="1"/>
-    <col min="20" max="20" width="86.28515625" customWidth="1"/>
-    <col min="21" max="21" width="105.85546875" customWidth="1"/>
-    <col min="22" max="22" width="70.42578125" customWidth="1"/>
+    <col min="13" max="13" width="19.26953125" customWidth="1"/>
+    <col min="14" max="14" width="15.7265625" customWidth="1"/>
+    <col min="15" max="15" width="13.54296875" customWidth="1"/>
+    <col min="16" max="16" width="12.54296875" customWidth="1"/>
+    <col min="17" max="17" width="23.26953125" customWidth="1"/>
+    <col min="18" max="18" width="30.54296875" customWidth="1"/>
+    <col min="19" max="19" width="16.7265625" customWidth="1"/>
+    <col min="20" max="20" width="86.26953125" customWidth="1"/>
+    <col min="21" max="21" width="105.81640625" customWidth="1"/>
+    <col min="22" max="22" width="70.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="42" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="42" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1631,7 +1920,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="58" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>90</v>
       </c>
@@ -1696,7 +1985,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="87" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>91</v>
       </c>
@@ -1761,7 +2050,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>6</v>
       </c>
@@ -1786,7 +2075,7 @@
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>8</v>
       </c>
@@ -1797,7 +2086,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1808,7 +2097,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="240" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>51</v>
       </c>
@@ -1852,7 +2141,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>55</v>
       </c>
@@ -1863,7 +2152,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="87" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>68</v>
       </c>
@@ -1908,7 +2197,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="87" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>76</v>
       </c>
@@ -1958,7 +2247,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>80</v>
       </c>
@@ -1970,7 +2259,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="210" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>86</v>
       </c>
@@ -2015,7 +2304,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="120" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="116" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>89</v>
       </c>
@@ -2057,7 +2346,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="120" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="116" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>109</v>
       </c>
@@ -2102,7 +2391,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>113</v>
       </c>
@@ -2114,7 +2403,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>183</v>
       </c>
@@ -2126,7 +2415,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>187</v>
       </c>
@@ -2138,7 +2427,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>188</v>
       </c>
@@ -2150,7 +2439,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>189</v>
       </c>
@@ -2162,7 +2451,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>199</v>
       </c>
@@ -2185,40 +2474,40 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B72208-97E1-4C7D-8DC1-CBFEC37313FA}">
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2:S2"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" customWidth="1"/>
+    <col min="7" max="7" width="23.81640625" customWidth="1"/>
+    <col min="8" max="8" width="18.26953125" customWidth="1"/>
+    <col min="9" max="9" width="25.7265625" customWidth="1"/>
+    <col min="10" max="10" width="16.81640625" customWidth="1"/>
+    <col min="11" max="11" width="18.453125" customWidth="1"/>
     <col min="12" max="12" width="33" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" customWidth="1"/>
-    <col min="17" max="17" width="23.28515625" customWidth="1"/>
-    <col min="18" max="18" width="30.5703125" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="19.26953125" customWidth="1"/>
+    <col min="14" max="14" width="15.7265625" customWidth="1"/>
+    <col min="15" max="15" width="13.54296875" customWidth="1"/>
+    <col min="16" max="16" width="12.54296875" customWidth="1"/>
+    <col min="17" max="17" width="23.26953125" customWidth="1"/>
+    <col min="18" max="18" width="30.54296875" customWidth="1"/>
+    <col min="19" max="19" width="16.7265625" customWidth="1"/>
     <col min="20" max="20" width="107" customWidth="1"/>
-    <col min="21" max="21" width="105.85546875" customWidth="1"/>
-    <col min="22" max="22" width="112.140625" customWidth="1"/>
+    <col min="21" max="21" width="105.81640625" customWidth="1"/>
+    <col min="22" max="22" width="112.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="42" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="42" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2286,10 +2575,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="2" customFormat="1" ht="240" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
+    <row r="2" spans="1:22" s="2" customFormat="1" ht="217.5" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>25</v>
       </c>
@@ -2336,7 +2622,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="255" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="246.5" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>37</v>
       </c>
@@ -2401,7 +2687,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="315" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="290" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>45</v>
       </c>
@@ -2466,7 +2752,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="180" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="174" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
@@ -2531,7 +2817,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="150" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="130.5" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>49</v>
       </c>
@@ -2596,7 +2882,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="150" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="130.5" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>49</v>
       </c>
@@ -2661,7 +2947,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="87" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>64</v>
       </c>
@@ -2726,7 +3012,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="270" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="261" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>74</v>
       </c>
@@ -2789,6 +3075,279 @@
       </c>
       <c r="V9" s="2" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" s="2" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>76</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <f t="shared" ref="B10:B13" si="0">"CAR-" &amp;A10&amp;"-24-DOT-INS"</f>
+        <v>CAR-76-24-DOT-INS</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="3">
+        <v>45911</v>
+      </c>
+      <c r="N10" s="3">
+        <v>45546</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="S10" s="2">
+        <v>3218284227</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" s="2" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>86</v>
+      </c>
+      <c r="B11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>CAR-86-24-DOT-INS</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" s="3">
+        <v>45911</v>
+      </c>
+      <c r="N11" s="3">
+        <v>45546</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="S11" s="2">
+        <v>3218284227</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" s="2" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>89</v>
+      </c>
+      <c r="B12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>CAR-89-24-DOT-INS</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" s="3">
+        <v>45911</v>
+      </c>
+      <c r="N12" s="3">
+        <v>45546</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="S12" s="2">
+        <v>3218284227</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" s="2" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>109</v>
+      </c>
+      <c r="B13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>CAR-109-24-DOT-INS</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M13" s="3">
+        <v>45911</v>
+      </c>
+      <c r="N13" s="3">
+        <v>45546</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="S13" s="2">
+        <v>3218284227</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2800,6 +3359,10 @@
     <hyperlink ref="R7" r:id="rId5" xr:uid="{3189892B-AC49-4B9C-BC6A-C75F8674D3C4}"/>
     <hyperlink ref="R8" r:id="rId6" xr:uid="{3FF560E3-7526-4BF1-80FC-F15FCB89C23D}"/>
     <hyperlink ref="R9" r:id="rId7" xr:uid="{7A755707-CA23-42B4-8F8F-A1C281B90C9C}"/>
+    <hyperlink ref="R10" r:id="rId8" xr:uid="{224FFEA1-7EC5-4788-93F5-6DE059FF57BE}"/>
+    <hyperlink ref="R11" r:id="rId9" xr:uid="{32020B44-8EEF-4FDB-BD4F-9EEAFFA3B3A2}"/>
+    <hyperlink ref="R12" r:id="rId10" xr:uid="{B8E7665E-CEB6-4242-845C-5B2D10044530}"/>
+    <hyperlink ref="R13" r:id="rId11" xr:uid="{3943FE55-A220-453F-A101-22FCFD5FD060}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2813,9 +3376,9 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="105" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="116" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>86</v>
       </c>
@@ -2866,7 +3429,7 @@
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
     </row>
-    <row r="2" spans="1:21" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
v1.4 Cambio de formato en Informe técnico
</commit_message>
<xml_diff>
--- a/basesDeDatos/baseDeDatosParaInforme.xlsx
+++ b/basesDeDatos/baseDeDatosParaInforme.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david.herrera\Proyectos_Codigos\automatizacionDocumental\basesDeDatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A9BCAF-877E-48F6-9153-66546437B144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8EAD85-3AFF-4D6B-B0D0-2A1FBD182439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="175">
   <si>
     <t>ITEM</t>
   </si>
@@ -552,17 +552,6 @@
     <t>Se hace la instalación del péndulo en el laboratorio de docencia en física del segundo piso. Se hacen pruebas de funcionamiento del motor. El motor funciona bajo los parámetros esperados. Se hacen pruebas del electroimán y se encuentra que genera fricción electromagnética según lo esperado. El péndulo presenta una ligera inclinación en su eje lo que causa que tenga fricción mecánica que no es ideal. Se hace el ajuste del eje para arreglar la inclinación del péndulo y se proceden a hacer pruebas de funcionamiento. El péndulo de torsión gira sin ninguna novedad y se hacen pruebas de ambas prácticas con éxito.</t>
   </si>
   <si>
-    <t>Los equipos se encuentran en su empaque original sin ningun signo de golpes, rayones o abolladuras. El embalaje se encuentra en buen estado. El equipo balístico (ambos) se encuentra en perfecto estado físico sin ninguna novedad estética. Todas las partes mecánicas se encuentran en buen estado incluyendo la escala angular y los disparadores. Los accesorios del kit se encuentran completos y se entrega todo el conjunto de tornillería y llaves bristol necesarias para el montaje.</t>
-  </si>
-  <si>
-    <t>Se recomienda almacenar los sensores cuando estén fuera de uso. El sensor debe estar desconectado en todo momento mientras que no esté en uso para no afectar su vida útil.
-Se recomienda cuidado con el almacenamiento del péndulo balístico, el cual se entrega en su empaque original para el mismo.
-Se recomienda almacenar los accesorios pequeños como las bolas en un lugar seguro para evitar extraviarlas. 
-Se recomienda no cambiar el computador en el cual se va a utilizar el software. Si se requiere hacer esto último, contactarnos para realizar este procedimiento. También, en caso de requerir instalar el software en más de un computador, lo cual es posible ya que se adquirieron dos licencias.
-Se recomienda almacenar el equipo en un lugar libre de polvo y humedad.
-Se recomienda hacer mantenimiento anual.</t>
-  </si>
-  <si>
     <t>Salomón Triana</t>
   </si>
   <si>
@@ -626,31 +615,7 @@
     <t>MULTÍMETRO DIGITAL DE REFERENCIA</t>
   </si>
   <si>
-    <t>INCUBADORA 161 L</t>
-  </si>
-  <si>
     <t>CABINA DE SEGURIDAD BIOLÓGICA</t>
-  </si>
-  <si>
-    <t>4:30pm</t>
-  </si>
-  <si>
-    <t>leidy.castillo@unad.edu.co</t>
-  </si>
-  <si>
-    <t>Los accesorios del kit se encuentran en perfectas condiciones. (bases, varillas, nueces y pinzas).
-Las bolas de acero y madera no presentan abolladuras. El disparador se encuentra en buenas condiciones estéticas.
-Los cronómetros 2-1 serial: 2303004005 y 2303004063 no presentan novedades estéticas y su empaque está en perfecto estado. 
-Ambas barreras fotoeléctricas se encuentran en su empaque sin novedades estéticas.</t>
-  </si>
-  <si>
-    <t>Se realiza el montaje del experimento siguiendo las guías experimentales de la marca.
-Se realiza la instalación de los cronómetros 2-1 utilizando las fuentes de 5V DC provistas.
-El cronómetro enciende correctamente.
-Se hace la instalación de las barreras fotoeléctricas y los ganchos de disparo en el montaje y se instalan en el cronómetro.
-Las barreras presentan condiciones funcionales óptimas y esperadas según los valores obtenidos en el cronómetro 2-1.
-Se hacen varias pruebas de lanzamiento obteniendo resultados experimentales para los tiempos de caida de la pelora menores a un segundo, lo cual es lo esperado.
-Midiendo la distancia entre los ganchos de disparo y la fotobarrera se hacen pruebas y cálculos de la constante de gravedad obteniendo en promedio un valor de 9.69m/s^2</t>
   </si>
   <si>
     <t>FLUKE</t>
@@ -676,16 +641,7 @@
 Conectar las entradas del multímetro correspondientes a la corriente máxima que se va a medir.</t>
   </si>
   <si>
-    <t>67.1</t>
-  </si>
-  <si>
-    <t>67.2</t>
-  </si>
-  <si>
     <t>67.3</t>
-  </si>
-  <si>
-    <t>Laboratorio Multipropósito 3</t>
   </si>
   <si>
     <t>Laboratorio Multipropósito 2</t>
@@ -697,9 +653,6 @@
 La base se encuentra embalada y no presenta novedades estéticas</t>
   </si>
   <si>
-    <t>MEMMERT</t>
-  </si>
-  <si>
     <t>TOPAIR</t>
   </si>
   <si>
@@ -707,12 +660,6 @@
   </si>
   <si>
     <t>21-455630</t>
-  </si>
-  <si>
-    <t>IN60</t>
-  </si>
-  <si>
-    <t>D521.0021</t>
   </si>
   <si>
     <t>1:30pm</t>
@@ -739,38 +686,79 @@
 </t>
   </si>
   <si>
+    <t>Leidy Castillos</t>
+  </si>
+  <si>
+    <t>leidy.castillos@unad.edu.co</t>
+  </si>
+  <si>
+    <t>SALA DE RADIOLOGIA</t>
+  </si>
+  <si>
+    <t>INS-008-23-CAR</t>
+  </si>
+  <si>
+    <t>Laboratorio Multipropósito 7</t>
+  </si>
+  <si>
+    <t>VER SECCIÓN VERIFICACIÓN</t>
+  </si>
+  <si>
     <t>NC</t>
   </si>
   <si>
-    <t>Equipo pendiente de instalación</t>
-  </si>
-  <si>
-    <t>El equipo se encuentra en el laboratorio ya desempaquetado y puesto en el lugar dispuesto para su instalación. Se encuentra en perfectas condiciones estéticas y no presenta abolladuras ni rayones.
-El cable se encuentra en perfecto estado estético.
-La incubadora no enciende después de conectada.</t>
-  </si>
-  <si>
-    <t>Se realiza la conexión del cable de poder de la incubadora.
-Al evidenciar que no enciende, se realiza apertura del equipo para revisar la electrónica interna.
-Después de varias verificaciones se encuentra que no hay contacto en dos de los fusibles.
-Se hace una conexión en puente con cable de cobre en lugar de los fusibles para verificar el correcto funcionamiento de la incubadora .
-La incubadora funciona con el puente de manera óptima. Se hace la desconexión de dichos puentes para evitar futuros daños por novedades eléctricas.</t>
-  </si>
-  <si>
-    <t>Electroequipos queda pendiente de hacer el reemplazo de los fusibles para que la incubadora funcione correctamente.
-Se recomienda no operar la incubadora por el momento.</t>
-  </si>
-  <si>
-    <t>Se realiza el desembalaje del kit para comprobar su estado inicial después del transporte. Se realiza una verificación del volumen de suministro de ambos kits para verificar la integridad de cada accesorio y la completitud de estos. Todos los accesorios se encuentran intactos. 
-Se realiza la instalación de ambas bases de la Unidad Balística con la tornillería y llave bristol provista. Se realiza la instalación de los sensores de velocidad en cada Unidad usando la tornillería provista. Se instalan las escala en el pié cónico. 
-Se hacen pruebas de las compuertas fotoeléctricas de los sensores de velocidad utilizando mediciones manuales y lanzamientos del disparador en 3 niveles. 
-Se hace la instalación de ambos péndulos balísticos en cada unidad y se realizan pruebas de lanzamiento de este para comprobar el funcionamiento mecánico de la trampa de proyectiles, los cuales demuestran funcionamiento óptimo. El indicador de altura del péndulo también funciona según lo esperado.
-Por último, se realiza la instalación del software MeasureDynamics en el computador provisto por la Universidad. Se entregan dos licencias con códigos: 92400121-440-17991601 y 92400121-440-16135891.
- El algoritmo de conversión y compresión de videos funcionan correctamente, y el análisis de video funciona perfectamente bajo parámetros recomendados.
-En general, el funcionamiento de todo el kit es óptimo y está listo para su uso.</t>
-  </si>
-  <si>
-    <t>Leidy Castillo</t>
+    <t>El equipo no funciona correctamente</t>
+  </si>
+  <si>
+    <t>Los equipos se encuentran en guacales posterior al transporte. Una vez removidos los guacales se hace una verificación estética de los equipos. No se presentan evidencias de golpes, rayones o abolladuras en la Unidad XR4.0. Los tubos de Rayos X presentan un estado estético óptimo, sin embargo presentan una ligera oxidación resultado del almacenamiento por un año aproximado. Los accesorios de análisis estructural y de tomografía computarizada se encuentran completos y en perfecto estado estético.
+El volumen de suministro contempla los siguientes elementos:
+Unidad de Rayos X Ref: 09057-99 Serial:132300652015
+Goniómetro Ref: 09057-10
+Tubo de Tungsteno Ref: 09057-80 Serial: 201100362845
+Tubo de Tungsteno Ref: 09057-80 Serial: 232300653644
+Kit de Tomografía CT Ref: 09180-88
+Kit de Análisis Estructural Ref: 09145-88
+ X-RAY SOPORTE UNIVERSALO DE CRISTALES PARA UNIDAD DE RAYOS X Ref: 09058-02
+X-RAY MODELO DE IMPLANTE PARA FOTOGRAFIA CON RAYOS X Ref: 09058-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las pruebas mencionadas se realizaron para cada tubo por aparte y en ambos se obtienen el mismo tipo de resultados ruidosos y de detección nula. La reinstalación del software se hizo dos veces. Al hacerla con permisos de administrador mejoraron unas configuraciones del protocolo de comunicación pero el sensor sigue sin mostrar exposición de radiación ionizante.
+Como diagnóstico es improbable que los tubos sean la causa del fallo ya que ambos tendrían que estar dañados y uno de ellos se sabe con seguridad que no ha sido manipulado ya que dejó las oficinas de Electroequipos apenas en septiembre 23 del 2024. Sin embargo, se tendrían que hacer pruebas con otros tubos y en otras unidades XR4.0 para descartar con seguridad del daño en los tubos.
+El Sensor XRIS no parece estar dañado puesto que enciende con normalidad y los drivers detectan correctamente la cámara para comunicarla al software measureCT.
+La unidad también parece tener buena comunicación con el software ya que se pueden cambiar los parámetros de voltaje y corriente desde el panel de control de la Unidad XR4.0 o desde el PC via el software. No obstante, esto no permite identificar la causa precisa del fallo. 
+A pesar de seguir las indicaciones sugeridas por los ingenieros de Phywe directamente,  no se logró indentificar la causa exacta del fallo, ni solucionarlo. Por ende se requiere de un apoyo más amplio y sólido por parte de fábrica.
+</t>
+  </si>
+  <si>
+    <t>Se realiza la remoción de los guacales.
+Se ubican los equipos en el laboratorio de Ciencias Radiológicas.
+Se realiza la instalación del software measure X-Ray y measureCT de Phywe con la licencia provista en la entrega.
+Se realiza la instalación de la cámara XRIS en la unidad. Se conecta a una fuente de poder externa de 12V para el encendido y via ethernet para el protocolo de comunicación al PC.
+La unidad se conecta via USB y el motor via conector Db15.
+Previo a las pruebas de comunicación se realiza la calibración de ambos tubos debido a que como han estado almacenados sin uso aproximadamente un año, presentan óxido. El óxido en un tubo de rayos X puede afectar la conductividad eléctrica, generar acumulación de calor y comprometer el vacío interno, lo que altera el flujo de corriente, la disipación del calor y la aceleración de electrones, resultando en un mal funcionamiento y menor precisión en la generación de rayos X.
+La calibración/activación inicial tiene una duración de una hora y se realiza según las indicaciones de los ingenieros de fábrica en Phywe así:
+Operar el equipo a 10kV-1mA por 10 minutos.
+Operar el equipo a 15kV-1mA por 10 minutos.
+Operar el equipo a 20kV-1mA por 10 minutos.
+Operar el equipo a 25kV-1mA por 10 minutos.
+Operar el equipo a 30kV-1mA por 10 minutos.
+Operar el equipo a 35kV-1mA por 10 minutos.
+Esto se hace para cada uno de los dos tubos. 
+Posteriormente se hace la calibración/activación final, la cual tiene una duración de 4.5 horas por cada tubo así:
+Operar el equipo a 10kV-1mA por 2 horas.
+Operar el equipo a 15kV-1mA por 30 minutos.
+Operar el equipo a 20kV-1mA por 30 minutos.
+Operar el equipo a 25kV-1mA por 30 minutos.
+Operar el equipo a 30kV-1mA por 30 minutos.
+Operar el equipo a 35kV-1mA por 30 minutos.
+Una vez hecho el anterior procedimiento se hacen pruebas de comunicación con el software measure CT. Al ejecutar el software se evidencia comunicación correcta con la unidad, el motor y la cámara.
+Se realiza la calibración de la cámara/detector y no se detecto exposición.
+Se inicia la vista en vivo y no se detecta exposición en la cámara. 
+Se realiza la calibración SSD y SOD y se intenta hacer nuevamente la calibración de la cámara, pero el detector aún no muestra ningún tipo de imagen de contraste.
+Se realiza una reinstalación del software y los drivers de la cámara como administrador.
+Se realizan las mismas pruebas anteriores sin éxito.
+Se realiza un cambio de configuración en el protocolo de comunicación, pero las pruebas siguen arrojando ruido.
+Las pruebas se realizan con la unidad vacía y con muestras, pero las imágenes obtenidas son exactamente iguales.</t>
   </si>
 </sst>
 </file>
@@ -1129,11 +1117,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{655EC420-93C8-4D5F-8A9C-EAA108D1F7F6}">
-  <dimension ref="A1:V37"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1221,34 +1209,30 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="2" customFormat="1" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>51</v>
-      </c>
-      <c r="B2" s="2" t="str">
-        <f>"CAR-" &amp;A2&amp;"-24-DOT-INS"</f>
-        <v>CAR-51-24-DOT-INS</v>
+    <row r="2" spans="1:22" s="2" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>166</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>34</v>
+        <v>169</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>169</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>23</v>
+        <v>170</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>23</v>
@@ -1257,452 +1241,90 @@
         <v>23</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>28</v>
+        <v>171</v>
       </c>
       <c r="M2" s="3">
-        <v>45924</v>
+        <v>45933</v>
       </c>
       <c r="N2" s="3">
-        <v>45559</v>
+        <v>45568</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>148</v>
+        <v>29</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="S2" s="2">
         <v>3042439787</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>135</v>
+        <v>172</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" s="2" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
-        <v>68</v>
-      </c>
-      <c r="B3" s="2" t="str">
-        <f t="shared" ref="B3:B8" si="0">"CAR-" &amp;A3&amp;"-24-DOT-INS"</f>
-        <v>CAR-68-24-DOT-INS</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" s="3">
-        <v>45924</v>
-      </c>
-      <c r="N3" s="3">
-        <v>45559</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="S3" s="2">
-        <v>3042439787</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" s="2" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>CAR-67.1-24-DOT-INS</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G4" s="2">
-        <v>65500090</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" s="3">
-        <v>45924</v>
-      </c>
-      <c r="N4" s="3">
-        <v>45559</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="S4" s="2">
-        <v>3042439787</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" s="2" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>CAR-67.2-24-DOT-INS</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G5" s="2">
-        <v>65500092</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M5" s="3">
-        <v>45925</v>
-      </c>
-      <c r="N5" s="3">
-        <v>45560</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="P5" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q5" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="S5" s="2">
-        <v>3042439787</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" s="2" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="B6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>CAR-67.3-24-DOT-INS</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G6" s="2">
-        <v>65350040</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M6" s="3">
-        <v>45925</v>
-      </c>
-      <c r="N6" s="3">
-        <v>45560</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="S6" s="2">
-        <v>3042439787</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" s="2" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="7">
-        <v>69</v>
-      </c>
-      <c r="B7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>CAR-69-24-DOT-INS</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="M7" s="3">
-        <v>45925</v>
-      </c>
-      <c r="N7" s="3">
-        <v>45560</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="R7" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="S7" s="2">
-        <v>3042439787</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="145" x14ac:dyDescent="0.35">
-      <c r="A8" s="7">
-        <v>117</v>
-      </c>
-      <c r="B8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>CAR-117-24-DOT-INS</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="G8" t="s">
-        <v>170</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M8" s="3">
-        <v>45925</v>
-      </c>
-      <c r="N8" s="3">
-        <v>45560</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="R8" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="S8" s="2">
-        <v>3042439787</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="V8" s="2" t="s">
-        <v>176</v>
-      </c>
+    </row>
+    <row r="3" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="R3" s="4"/>
+    </row>
+    <row r="4" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="R5" s="4"/>
+    </row>
+    <row r="6" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="R6" s="4"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A7" s="7"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B9" s="2"/>
@@ -1787,19 +1409,10 @@
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B37" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="R2" r:id="rId1" xr:uid="{F8E6D1E9-1553-474E-9800-4CD0D2FB6D00}"/>
-    <hyperlink ref="R3" r:id="rId2" xr:uid="{52F1C42E-D920-4F2E-BC75-49B0555CD2F7}"/>
-    <hyperlink ref="R4" r:id="rId3" xr:uid="{AA28332A-5A72-4F1B-915C-1D59FC4B1516}"/>
-    <hyperlink ref="R5" r:id="rId4" xr:uid="{AAB82298-B14E-4984-9FFB-C1BEB7E5C1CC}"/>
-    <hyperlink ref="R6" r:id="rId5" xr:uid="{D0EBCE4C-E78A-4891-B7C4-91EA4F281AD0}"/>
-    <hyperlink ref="R7" r:id="rId6" xr:uid="{23599907-B198-44F5-8B30-C65E900ECF7A}"/>
-    <hyperlink ref="R8" r:id="rId7" xr:uid="{D0023600-EDFF-42FE-A2EC-C9DB695A7F60}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1819,11 +1432,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V20"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2415,7 +2028,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>187</v>
       </c>
@@ -2427,7 +2040,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>188</v>
       </c>
@@ -2439,7 +2052,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>189</v>
       </c>
@@ -2451,7 +2064,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>199</v>
       </c>
@@ -2461,12 +2074,152 @@
       </c>
       <c r="C20" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" s="2" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B21" s="2" t="str">
+        <f t="shared" ref="B21:B22" si="1">"CAR-" &amp;A21&amp;"-24-DOT-INS"</f>
+        <v>CAR-67.3-24-DOT-INS</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G21" s="2">
+        <v>65350040</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M21" s="3">
+        <v>45925</v>
+      </c>
+      <c r="N21" s="3">
+        <v>45560</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="S21" s="2">
+        <v>3042439787</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="U21" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="V21" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="145" x14ac:dyDescent="0.35">
+      <c r="A22" s="7">
+        <v>117</v>
+      </c>
+      <c r="B22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>CAR-117-24-DOT-INS</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G22" t="s">
+        <v>159</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M22" s="3">
+        <v>45925</v>
+      </c>
+      <c r="N22" s="3">
+        <v>45560</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="S22" s="2">
+        <v>3042439787</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="U22" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="V22" s="2" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="R3" r:id="rId1" xr:uid="{4AF0BF26-BF9A-4D7D-A4D9-D053EA8BA2BF}"/>
     <hyperlink ref="R2" r:id="rId2" xr:uid="{A1EB34BD-0937-4458-9008-C393DAC213D7}"/>
+    <hyperlink ref="R21" r:id="rId3" xr:uid="{F6CAE53A-9D85-435E-B5CA-23158DB1446A}"/>
+    <hyperlink ref="R22" r:id="rId4" xr:uid="{80086CB2-0AD2-46F2-8953-A6DFA6001394}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3089,7 +2842,7 @@
         <v>65</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>67</v>
@@ -3119,16 +2872,16 @@
         <v>45546</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>30</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="S10" s="2">
         <v>3218284227</v>
@@ -3155,7 +2908,7 @@
         <v>98</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>51</v>
@@ -3188,16 +2941,16 @@
         <v>45546</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="S11" s="2">
         <v>3218284227</v>
@@ -3206,7 +2959,7 @@
         <v>112</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V11" s="2" t="s">
         <v>114</v>
@@ -3224,7 +2977,7 @@
         <v>99</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>22</v>
@@ -3257,16 +3010,16 @@
         <v>45546</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="S12" s="2">
         <v>3218284227</v>
@@ -3275,7 +3028,7 @@
         <v>124</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="V12" s="2" t="s">
         <v>126</v>
@@ -3293,7 +3046,7 @@
         <v>100</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>22</v>
@@ -3326,28 +3079,28 @@
         <v>45546</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="S13" s="2">
         <v>3218284227</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>